<commit_message>
Removed track actual order and track duration
</commit_message>
<xml_diff>
--- a/V1/Dataset/N2OR_New.xlsx
+++ b/V1/Dataset/N2OR_New.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\V1\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AA2CE5-E4DF-4888-ADBD-A2E56A002F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE602F8-A456-4368-98B0-B968BF84B63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="22" r:id="rId1"/>
@@ -52,7 +52,7 @@
     <author>ΓΙΑΡΟΣΛΑΒ ΠΙΛΙΑΒΣΚΙ</author>
   </authors>
   <commentList>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{67F9A09A-505A-46DA-9298-8A8AA994B592}">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{67F9A09A-505A-46DA-9298-8A8AA994B592}">
       <text>
         <r>
           <rPr>
@@ -782,7 +782,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D6C26095-3954-4DE8-B600-49D1FC1771E2}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D6C26095-3954-4DE8-B600-49D1FC1771E2}">
       <text>
         <r>
           <rPr>
@@ -1737,7 +1737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="296">
   <si>
     <t>Metaheuristics</t>
   </si>
@@ -2425,9 +2425,6 @@
   </si>
   <si>
     <t>Attendees Conflicts:</t>
-  </si>
-  <si>
-    <t>Track Duration:</t>
   </si>
   <si>
     <t>This spreadsheet contains the necessary inputs for the Conference Scheduler and allows the user to make configurations. It consists of the following sheets: submissions, tracks, sessions, rooms, tracks_sessions|penalty, tracks_rooms|penalty, tracks_tracks|penalty, and sessions_rooms|penalty.</t>
@@ -2711,9 +2708,6 @@
   </si>
   <si>
     <t>Tracks Relative Order:</t>
-  </si>
-  <si>
-    <t>Tracks Actual Order:</t>
   </si>
   <si>
     <t>Tracks Same Room</t>
@@ -3381,18 +3375,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3402,6 +3384,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3410,12 +3398,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3429,10 +3411,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3449,9 +3443,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3474,14 +3465,17 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3498,10 +3492,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3804,7 +3794,7 @@
     </row>
     <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -3854,8 +3844,8 @@
       <c r="E10" s="52"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="60" t="s">
-        <v>112</v>
+      <c r="A11" s="59" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -3877,347 +3867,347 @@
       <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="41"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="58"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="59"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
     </row>
     <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="56"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="61"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="34"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="61"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="61"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="62" t="s">
+      <c r="A33" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="43"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="42"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="43"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="42"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="43"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="42"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="43"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="42"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="43"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="42"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="43"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="42"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="43"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="38"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="39"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="37"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="37"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="41"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="32"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="31"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="32"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="32"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="32"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="39"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="37"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="37"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="41"/>
+    </row>
+    <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="60"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="61"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="48"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="48"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="63"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="62"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="63"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="62"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="63"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="62"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="63"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="62"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="63"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="62"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="63"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="62"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="63"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="42"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="43"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="45"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="36"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="36"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="36"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="36"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="42"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="43"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="39"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="38"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="39"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="45"/>
-    </row>
-    <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="33"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="34"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="48"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="34"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="48"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="32"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="33"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="61"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="33"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="61"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="29" t="s">
@@ -4226,427 +4216,439 @@
       <c r="E57" s="20"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="36"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="35"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="36"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="32"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="40" t="s">
+      <c r="A60" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="41"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="45"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="40"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="41"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="45"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="40"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="41"/>
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="45"/>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="42"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="42"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="43"/>
+      <c r="A63" s="38"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="39"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="37" t="s">
+      <c r="A64" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="39"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="37"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="38"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="39"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="37"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="44"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="45"/>
+      <c r="A66" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="41"/>
     </row>
     <row r="67" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="33"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="60"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="61"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="31"/>
+      <c r="A68" s="46"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="47"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="37" t="s">
+      <c r="A69" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="38"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="39"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="37"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="38"/>
-      <c r="B70" s="38"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="38"/>
-      <c r="E70" s="39"/>
+      <c r="A70" s="36"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="37"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="40" t="s">
+      <c r="A71" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="41"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="45"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="40"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="41"/>
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="45"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="40"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="41"/>
+      <c r="A73" s="44"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="45"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="40"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="41"/>
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="45"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="40"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="41"/>
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="45"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="40"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="41"/>
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="45"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="40"/>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="41"/>
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="45"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="40"/>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="41"/>
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="45"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="46"/>
-      <c r="B79" s="46"/>
-      <c r="C79" s="46"/>
-      <c r="D79" s="46"/>
-      <c r="E79" s="47"/>
+      <c r="A79" s="62"/>
+      <c r="B79" s="62"/>
+      <c r="C79" s="62"/>
+      <c r="D79" s="62"/>
+      <c r="E79" s="63"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="37" t="s">
+      <c r="A80" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="38"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="39"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="37"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="38"/>
-      <c r="B81" s="38"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="39"/>
+      <c r="A81" s="36"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="37"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="40" t="s">
+      <c r="A82" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="40"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="40"/>
-      <c r="E82" s="41"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="45"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="40"/>
-      <c r="B83" s="40"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="40"/>
-      <c r="E83" s="41"/>
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="45"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="40"/>
-      <c r="B84" s="40"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="41"/>
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="45"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="40"/>
-      <c r="B85" s="40"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="45"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="40"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="41"/>
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="45"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="40"/>
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="41"/>
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="45"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="40"/>
-      <c r="B88" s="40"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="40"/>
-      <c r="E88" s="41"/>
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="45"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="40"/>
-      <c r="B89" s="40"/>
-      <c r="C89" s="40"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="41"/>
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="45"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="31"/>
+      <c r="A90" s="46"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="46"/>
+      <c r="D90" s="46"/>
+      <c r="E90" s="47"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="37" t="s">
+      <c r="A91" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="B91" s="38"/>
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="39"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="37"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="38"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="39"/>
+      <c r="A92" s="36"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="36"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="37"/>
     </row>
     <row r="93" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="40" t="s">
+      <c r="A93" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B93" s="40"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="41"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="45"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="40"/>
-      <c r="B94" s="40"/>
-      <c r="C94" s="40"/>
-      <c r="D94" s="40"/>
-      <c r="E94" s="41"/>
+      <c r="A94" s="44"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="45"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="40"/>
-      <c r="B95" s="40"/>
-      <c r="C95" s="40"/>
-      <c r="D95" s="40"/>
-      <c r="E95" s="41"/>
+      <c r="A95" s="44"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="45"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="40"/>
-      <c r="B96" s="40"/>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-      <c r="E96" s="41"/>
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="45"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="40"/>
-      <c r="B97" s="40"/>
-      <c r="C97" s="40"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="41"/>
+      <c r="A97" s="44"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="45"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="40"/>
-      <c r="B98" s="40"/>
-      <c r="C98" s="40"/>
-      <c r="D98" s="40"/>
-      <c r="E98" s="41"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="45"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="40"/>
-      <c r="B99" s="40"/>
-      <c r="C99" s="40"/>
-      <c r="D99" s="40"/>
-      <c r="E99" s="41"/>
+      <c r="A99" s="44"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="45"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="40"/>
-      <c r="B100" s="40"/>
-      <c r="C100" s="40"/>
-      <c r="D100" s="40"/>
-      <c r="E100" s="41"/>
+      <c r="A100" s="44"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="45"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="30"/>
-      <c r="B101" s="30"/>
-      <c r="C101" s="30"/>
-      <c r="D101" s="30"/>
-      <c r="E101" s="31"/>
+      <c r="A101" s="46"/>
+      <c r="B101" s="46"/>
+      <c r="C101" s="46"/>
+      <c r="D101" s="46"/>
+      <c r="E101" s="47"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="37" t="s">
+      <c r="A102" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B102" s="38"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="39"/>
+      <c r="B102" s="36"/>
+      <c r="C102" s="36"/>
+      <c r="D102" s="36"/>
+      <c r="E102" s="37"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="38"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="39"/>
+      <c r="A103" s="36"/>
+      <c r="B103" s="36"/>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="37"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="40" t="s">
+      <c r="A104" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B104" s="40"/>
-      <c r="C104" s="40"/>
-      <c r="D104" s="40"/>
-      <c r="E104" s="41"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="45"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="40"/>
-      <c r="B105" s="40"/>
-      <c r="C105" s="40"/>
-      <c r="D105" s="40"/>
-      <c r="E105" s="41"/>
+      <c r="A105" s="44"/>
+      <c r="B105" s="44"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="44"/>
+      <c r="E105" s="45"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="40"/>
-      <c r="B106" s="40"/>
-      <c r="C106" s="40"/>
-      <c r="D106" s="40"/>
-      <c r="E106" s="41"/>
+      <c r="A106" s="44"/>
+      <c r="B106" s="44"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="44"/>
+      <c r="E106" s="45"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="40"/>
-      <c r="B107" s="40"/>
-      <c r="C107" s="40"/>
-      <c r="D107" s="40"/>
-      <c r="E107" s="41"/>
+      <c r="A107" s="44"/>
+      <c r="B107" s="44"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="44"/>
+      <c r="E107" s="45"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="40"/>
-      <c r="B108" s="40"/>
-      <c r="C108" s="40"/>
-      <c r="D108" s="40"/>
-      <c r="E108" s="41"/>
+      <c r="A108" s="44"/>
+      <c r="B108" s="44"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="44"/>
+      <c r="E108" s="45"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" s="40"/>
-      <c r="B109" s="40"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="40"/>
-      <c r="E109" s="41"/>
+      <c r="A109" s="44"/>
+      <c r="B109" s="44"/>
+      <c r="C109" s="44"/>
+      <c r="D109" s="44"/>
+      <c r="E109" s="45"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="40"/>
-      <c r="B110" s="40"/>
-      <c r="C110" s="40"/>
-      <c r="D110" s="40"/>
-      <c r="E110" s="41"/>
+      <c r="A110" s="44"/>
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="45"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="40"/>
-      <c r="B111" s="40"/>
-      <c r="C111" s="40"/>
-      <c r="D111" s="40"/>
-      <c r="E111" s="41"/>
+      <c r="A111" s="44"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="45"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="30"/>
-      <c r="B112" s="30"/>
-      <c r="C112" s="30"/>
-      <c r="D112" s="30"/>
-      <c r="E112" s="31"/>
+      <c r="A112" s="46"/>
+      <c r="B112" s="46"/>
+      <c r="C112" s="46"/>
+      <c r="D112" s="46"/>
+      <c r="E112" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A44:E45"/>
-    <mergeCell ref="A46:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A41:E42"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E39"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A58:E59"/>
+    <mergeCell ref="A91:E92"/>
+    <mergeCell ref="A93:E100"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A69:E70"/>
+    <mergeCell ref="A60:E62"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A64:E65"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A71:E78"/>
+    <mergeCell ref="A102:E103"/>
+    <mergeCell ref="A104:E111"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A79:E79"/>
     <mergeCell ref="A80:E81"/>
     <mergeCell ref="A82:E89"/>
     <mergeCell ref="A90:E90"/>
@@ -4663,27 +4665,15 @@
     <mergeCell ref="A20:E21"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A27:E29"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A58:E59"/>
-    <mergeCell ref="A91:E92"/>
-    <mergeCell ref="A93:E100"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="A69:E70"/>
-    <mergeCell ref="A60:E62"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A64:E65"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A71:E78"/>
-    <mergeCell ref="A102:E103"/>
-    <mergeCell ref="A104:E111"/>
+    <mergeCell ref="A44:E45"/>
+    <mergeCell ref="A46:E47"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A41:E42"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4929,10 +4919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B4773B-09CB-4AE1-B7A2-EA1A4F4D3191}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4967,7 +4957,7 @@
         <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>99</v>
@@ -4985,7 +4975,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -4999,7 +4989,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="27">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -5013,7 +5003,7 @@
         <v>102</v>
       </c>
       <c r="E5" s="27">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -5021,7 +5011,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="27">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -5029,7 +5019,7 @@
         <v>104</v>
       </c>
       <c r="E7" s="27">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -5037,103 +5027,103 @@
         <v>105</v>
       </c>
       <c r="E8" s="27">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D9" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9" s="27">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D10" s="23" t="s">
-        <v>184</v>
+        <v>268</v>
       </c>
       <c r="E10" s="27">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11" s="23" t="s">
-        <v>270</v>
+        <v>181</v>
       </c>
       <c r="E11" s="27">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D12" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E12" s="27">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13" s="23" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
       <c r="E13" s="27">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D14" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E14" s="27">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D15" s="23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E15" s="27">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D16" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E16" s="27">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D17" s="23" t="s">
-        <v>109</v>
+        <v>171</v>
       </c>
       <c r="E17" s="27">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D18" s="23" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E18" s="27">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D19" s="23" t="s">
-        <v>110</v>
+        <v>185</v>
       </c>
       <c r="E19" s="27">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D20" s="23" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E20" s="27">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.3">
@@ -5141,55 +5131,55 @@
         <v>187</v>
       </c>
       <c r="E21" s="27">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D22" s="23" t="s">
-        <v>188</v>
+        <v>259</v>
       </c>
       <c r="E22" s="27">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D23" s="23" t="s">
-        <v>189</v>
+        <v>260</v>
       </c>
       <c r="E23" s="27">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D24" s="23" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E24" s="27">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D25" s="23" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E25" s="27">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D26" s="23" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E26" s="27">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D27" s="23" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E27" s="27">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.3">
@@ -5197,7 +5187,7 @@
         <v>263</v>
       </c>
       <c r="E28" s="27">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.3">
@@ -5205,7 +5195,7 @@
         <v>264</v>
       </c>
       <c r="E29" s="27">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.3">
@@ -5213,7 +5203,7 @@
         <v>265</v>
       </c>
       <c r="E30" s="27">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.3">
@@ -5221,23 +5211,7 @@
         <v>266</v>
       </c>
       <c r="E31" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D32" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="E32" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D33" s="23" t="s">
-        <v>268</v>
-      </c>
-      <c r="E33" s="27">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5253,8 +5227,8 @@
   <dimension ref="A1:T157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15:B18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5274,7 +5248,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="7" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>48</v>
@@ -5283,22 +5257,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>166</v>
-      </c>
       <c r="H1" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>50</v>
@@ -5356,10 +5330,10 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -5392,7 +5366,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K3" s="9"/>
       <c r="P3" s="1"/>
@@ -5426,7 +5400,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K4" s="9"/>
       <c r="P4" s="1"/>
@@ -5460,10 +5434,10 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -5496,7 +5470,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K6" s="9"/>
       <c r="P6" s="1"/>
@@ -5530,7 +5504,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K7" s="9"/>
       <c r="P7" s="1"/>
@@ -5564,7 +5538,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K8" s="9"/>
       <c r="N8" s="1">
@@ -5604,7 +5578,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K9" s="9"/>
       <c r="P9" s="1"/>
@@ -5638,10 +5612,10 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -5674,7 +5648,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K11" s="9"/>
       <c r="P11" s="1"/>
@@ -5708,7 +5682,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="1">
@@ -5748,7 +5722,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="1">
@@ -5788,7 +5762,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K14" s="9"/>
       <c r="P14" s="1"/>
@@ -5822,7 +5796,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K15" s="9"/>
       <c r="P15" s="1"/>
@@ -5856,10 +5830,10 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -5892,7 +5866,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K17" s="9"/>
       <c r="P17" s="1"/>
@@ -5926,7 +5900,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K18" s="9"/>
       <c r="P18" s="1"/>
@@ -5960,7 +5934,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N19" s="1">
         <v>1</v>
@@ -5998,7 +5972,7 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -6030,10 +6004,10 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -6065,10 +6039,10 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -6100,7 +6074,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -6132,7 +6106,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K24" s="9"/>
       <c r="P24" s="1"/>
@@ -6165,7 +6139,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K25" s="9"/>
       <c r="P25" s="1"/>
@@ -6198,7 +6172,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K26" s="9"/>
       <c r="P26" s="1"/>
@@ -6231,7 +6205,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K27" s="9"/>
       <c r="P27" s="1"/>
@@ -6266,10 +6240,10 @@
         <v>36</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -6278,7 +6252,7 @@
     </row>
     <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>11</v>
@@ -6301,7 +6275,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N29" s="1">
         <v>1</v>
@@ -6339,7 +6313,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -6370,7 +6344,7 @@
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -6402,10 +6376,10 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -6437,7 +6411,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K33" s="9"/>
       <c r="P33" s="1"/>
@@ -6470,7 +6444,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K34" s="9"/>
       <c r="P34" s="1"/>
@@ -6503,7 +6477,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K35" s="9"/>
       <c r="P35" s="1"/>
@@ -6536,7 +6510,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -7089,51 +7063,48 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.21875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="6"/>
+    <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.33203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>170</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -7146,11 +7117,8 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -7163,14 +7131,11 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -7183,12 +7148,9 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -7201,14 +7163,11 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -7221,13 +7180,10 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -7235,18 +7191,15 @@
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
         <v>100</v>
       </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -7259,13 +7212,10 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -7278,106 +7228,102 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H34" s="9"/>
-    </row>
-    <row r="35" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="8:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="9"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="7:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -7406,43 +7352,43 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>164</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>52</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
@@ -7450,13 +7396,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>1</v>
@@ -7464,10 +7410,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>88</v>
@@ -7478,13 +7424,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>1</v>
@@ -7492,13 +7438,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>1</v>
@@ -7506,13 +7452,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I7" s="1" t="b">
         <v>1</v>
@@ -7520,13 +7466,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I8" s="1" t="b">
         <v>1</v>
@@ -7534,13 +7480,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I9" s="1" t="b">
         <v>1</v>
@@ -7548,13 +7494,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I10" s="1" t="b">
         <v>1</v>
@@ -7562,13 +7508,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I11" s="1" t="b">
         <v>1</v>
@@ -7576,13 +7522,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I12" s="1" t="b">
         <v>1</v>
@@ -7590,13 +7536,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I13" s="1" t="b">
         <v>1</v>
@@ -7604,13 +7550,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I14" s="1" t="b">
         <v>1</v>
@@ -7618,13 +7564,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I15" s="1" t="b">
         <v>1</v>
@@ -7632,13 +7578,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I16" s="1" t="b">
         <v>1</v>
@@ -7646,13 +7592,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I17" s="1" t="b">
         <v>1</v>
@@ -7660,13 +7606,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I18" s="1" t="b">
         <v>1</v>
@@ -7674,13 +7620,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I19" s="1" t="b">
         <v>1</v>
@@ -7688,13 +7634,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I20" s="1" t="b">
         <v>1</v>
@@ -7702,13 +7648,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>1</v>
@@ -7716,13 +7662,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I22" s="1" t="b">
         <v>1</v>
@@ -7730,13 +7676,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I23" s="1" t="b">
         <v>1</v>
@@ -7744,13 +7690,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I24" s="1" t="b">
         <v>1</v>
@@ -7758,13 +7704,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I25" s="1" t="b">
         <v>1</v>
@@ -7772,13 +7718,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I26" s="1" t="b">
         <v>1</v>
@@ -7786,13 +7732,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I27" s="1" t="b">
         <v>1</v>
@@ -7800,13 +7746,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I28" s="1" t="b">
         <v>1</v>
@@ -7814,13 +7760,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I29" s="1" t="b">
         <v>1</v>
@@ -7828,13 +7774,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I30" s="1" t="b">
         <v>1</v>
@@ -7842,13 +7788,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I31" s="1" t="b">
         <v>1</v>
@@ -7856,13 +7802,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I32" s="1" t="b">
         <v>1</v>
@@ -7870,13 +7816,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I33" s="1" t="b">
         <v>1</v>
@@ -7884,13 +7830,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I34" s="1" t="b">
         <v>1</v>
@@ -7898,13 +7844,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I35" s="1" t="b">
         <v>1</v>
@@ -7912,13 +7858,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I36" s="1" t="b">
         <v>1</v>
@@ -7926,13 +7872,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I37" s="1" t="b">
         <v>1</v>
@@ -7940,13 +7886,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I38" s="1" t="b">
         <v>1</v>
@@ -7954,13 +7900,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I39" s="1" t="b">
         <v>1</v>
@@ -7968,13 +7914,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I40" s="1" t="b">
         <v>1</v>
@@ -7982,13 +7928,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I41" s="1" t="b">
         <v>1</v>
@@ -7996,13 +7942,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I42" s="1" t="b">
         <v>1</v>
@@ -8010,13 +7956,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I43" s="1" t="b">
         <v>1</v>
@@ -8024,13 +7970,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I44" s="1" t="b">
         <v>1</v>
@@ -8038,13 +7984,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I45" s="1" t="b">
         <v>1</v>
@@ -8052,13 +7998,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I46" s="1" t="b">
         <v>1</v>
@@ -8066,13 +8012,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I47" s="1" t="b">
         <v>1</v>
@@ -8080,13 +8026,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I48" s="1" t="b">
         <v>1</v>
@@ -8094,13 +8040,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I49" s="1" t="b">
         <v>1</v>
@@ -8108,13 +8054,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I50" s="1" t="b">
         <v>1</v>
@@ -8122,13 +8068,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I51" s="1" t="b">
         <v>1</v>
@@ -8136,13 +8082,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I52" s="1" t="b">
         <v>1</v>
@@ -8150,13 +8096,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I53" s="1" t="b">
         <v>1</v>
@@ -8189,13 +8135,13 @@
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>49</v>
@@ -8360,10 +8306,10 @@
   <sheetData>
     <row r="1" spans="1:19" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -8388,7 +8334,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8396,7 +8342,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8404,7 +8350,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8412,7 +8358,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>